<commit_message>
Adding manually curated data
</commit_message>
<xml_diff>
--- a/Data/phenotypic data/RawData/2012 Data/BogLower5-R6 (Parents).xlsx
+++ b/Data/phenotypic data/RawData/2012 Data/BogLower5-R6 (Parents).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="400" windowWidth="27560" windowHeight="17840"/>
+    <workbookView xWindow="720" yWindow="400" windowWidth="25440" windowHeight="17840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1772,7 +1772,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="22">
         <v>2</v>

</xml_diff>